<commit_message>
Basic UIBank Cases done
</commit_message>
<xml_diff>
--- a/TestDataExample.xlsx
+++ b/TestDataExample.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
   <si>
     <t>AccountName</t>
   </si>
@@ -42,6 +42,15 @@
   </si>
   <si>
     <t>Test Account</t>
+  </si>
+  <si>
+    <t>CredentialName</t>
+  </si>
+  <si>
+    <t>CredentialUIBANK</t>
+  </si>
+  <si>
+    <t>CredentialUIBANKNODATA</t>
   </si>
 </sst>
 </file>
@@ -359,10 +368,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -371,7 +380,7 @@
     <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -381,8 +390,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -392,8 +404,11 @@
       <c r="C2">
         <v>100</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -403,8 +418,11 @@
       <c r="C3">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -414,8 +432,54 @@
       <c r="C4">
         <v>-1</v>
       </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>-1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>-1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>-1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>